<commit_message>
Update to include OLS on spreadsheet
</commit_message>
<xml_diff>
--- a/doc/AlgorithmMetricsData.xlsx
+++ b/doc/AlgorithmMetricsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsill\Desktop\python-projects\CS490LDA-Project1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335AD7E9-D328-40F2-9E8E-2466830858D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E675D234-1F31-4FB1-9147-2E463D6AD033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{A14A169C-2F58-45F0-A0FE-0DCDA8B376A8}"/>
+    <workbookView xWindow="9195" yWindow="4215" windowWidth="28800" windowHeight="15435" xr2:uid="{A14A169C-2F58-45F0-A0FE-0DCDA8B376A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Model</t>
   </si>
@@ -163,6 +163,42 @@
   </si>
   <si>
     <t>2148.72 kB</t>
+  </si>
+  <si>
+    <t>10 Lin Regs</t>
+  </si>
+  <si>
+    <t>1 Lin Reg</t>
+  </si>
+  <si>
+    <t>100 Lin Regs</t>
+  </si>
+  <si>
+    <t>0.00729 s</t>
+  </si>
+  <si>
+    <t>0.00838 s</t>
+  </si>
+  <si>
+    <t>0.0297 s</t>
+  </si>
+  <si>
+    <t>0.0365 ms</t>
+  </si>
+  <si>
+    <t>0.0433 ms</t>
+  </si>
+  <si>
+    <t>0.0763 ms</t>
+  </si>
+  <si>
+    <t>0.0156 kB</t>
+  </si>
+  <si>
+    <t>0.234 kB</t>
+  </si>
+  <si>
+    <t>2.344 kB</t>
   </si>
 </sst>
 </file>
@@ -237,7 +273,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -248,14 +286,16 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,15 +307,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,16 +640,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE73A122-1229-47E6-B331-9182E99757EE}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="20.140625" style="2" customWidth="1"/>
@@ -647,25 +695,25 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1">
         <v>24.103000000000002</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <v>22.044</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -676,25 +724,25 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>24.372</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>21.92</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -705,25 +753,25 @@
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="1">
         <v>25.259</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>31.277999999999999</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -734,56 +782,111 @@
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="1">
         <v>25.991</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>30.759</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>15.632999999999999</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>13.864000000000001</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="12">
+        <v>14.4</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="12">
+        <v>14.43</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13">
+        <v>6.39</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>